<commit_message>
updated videos to 2024
</commit_message>
<xml_diff>
--- a/backend/data/TranslatedContent.xlsx
+++ b/backend/data/TranslatedContent.xlsx
@@ -1396,57 +1396,49 @@
     <t>step1VideoID</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <u val="single"/>
-        <sz val="13"/>
-        <color indexed="16"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>bakLU5yKezs</t>
-    </r>
-  </si>
-  <si>
-    <t>KVaRgbKBOSw</t>
-  </si>
-  <si>
-    <t>pIJ2ecJS-ws</t>
-  </si>
-  <si>
-    <t>xgHVWwLK1o4</t>
-  </si>
-  <si>
-    <t>h6NtwuB5CHw</t>
-  </si>
-  <si>
-    <t>-oRwYZ24UII</t>
-  </si>
-  <si>
-    <t>eFDm9db8Jzc</t>
-  </si>
-  <si>
-    <t>R2F6YqFSq-Q</t>
-  </si>
-  <si>
-    <t>QGlTwRcG-Fg</t>
-  </si>
-  <si>
-    <t>LIruW6czK3Y</t>
-  </si>
-  <si>
-    <t>FcwrJr61Hac</t>
+    <t>kGIkFU92Q6s</t>
+  </si>
+  <si>
+    <t>UI7OVfyWPLQ</t>
+  </si>
+  <si>
+    <t>T88sb7BZ0O0</t>
+  </si>
+  <si>
+    <t>w3m3gTSHcHo</t>
+  </si>
+  <si>
+    <t>tANLqtR_mNk</t>
+  </si>
+  <si>
+    <t>z55c4TkwcRU</t>
+  </si>
+  <si>
+    <t>UuOfOm6pBio</t>
+  </si>
+  <si>
+    <t>vEgHnkjI584</t>
+  </si>
+  <si>
+    <t>10XhFzGML1k</t>
+  </si>
+  <si>
+    <t>YPeL0-mFZ9I</t>
+  </si>
+  <si>
+    <t>fsI5YKXelqE</t>
   </si>
   <si>
     <t>CmxL0DdGVDE</t>
   </si>
   <si>
-    <t>aH13Ql4DD4s</t>
-  </si>
-  <si>
-    <t>A_fB7gGGr88</t>
-  </si>
-  <si>
-    <t>VY6aoemzpsg</t>
+    <t>BYxYHuwcrus</t>
+  </si>
+  <si>
+    <t>1p7b1ZPoFAc</t>
+  </si>
+  <si>
+    <t>1h85LFO4rD4</t>
   </si>
   <si>
     <t>step1Tip1</t>
@@ -2915,7 +2907,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="17"/>
+        <color indexed="16"/>
         <rFont val="Arial"/>
       </rPr>
       <t>2024</t>
@@ -3192,7 +3184,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3211,7 +3203,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3230,7 +3222,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3249,7 +3241,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3268,7 +3260,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3287,7 +3279,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3314,7 +3306,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3333,7 +3325,7 @@
       <rPr>
         <u val="single"/>
         <sz val="18"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3352,7 +3344,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3371,7 +3363,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3398,7 +3390,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3425,7 +3417,7 @@
       <rPr>
         <u val="single"/>
         <sz val="16"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3452,7 +3444,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3479,7 +3471,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3539,7 +3531,7 @@
       <rPr>
         <u val="single"/>
         <sz val="13"/>
-        <color indexed="16"/>
+        <color indexed="17"/>
         <rFont val="Arial"/>
       </rPr>
       <t>www.e-immigrate.info</t>
@@ -3569,7 +3561,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="17"/>
+        <color indexed="16"/>
         <rFont val="Arial"/>
       </rPr>
       <t>2024</t>
@@ -3598,7 +3590,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="17"/>
+        <color indexed="16"/>
         <rFont val="Arial"/>
       </rPr>
       <t>2024</t>
@@ -3619,7 +3611,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="17"/>
+        <color indexed="16"/>
         <rFont val="Arial"/>
       </rPr>
       <t>2024</t>
@@ -3692,7 +3684,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="17"/>
+        <color indexed="16"/>
         <rFont val="Arial"/>
       </rPr>
       <t>May 16th</t>
@@ -3721,7 +3713,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="17"/>
+        <color indexed="16"/>
         <rFont val="Arial"/>
       </rPr>
       <t>accredited legal representatives</t>
@@ -3742,7 +3734,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="17"/>
+        <color indexed="16"/>
         <rFont val="Arial"/>
       </rPr>
       <t>If your case is too complex for our workshop, we will follow up with you by email no later than Tuesday, May 31th.</t>
@@ -3761,7 +3753,7 @@
     <r>
       <rPr>
         <sz val="10"/>
-        <color indexed="17"/>
+        <color indexed="16"/>
         <rFont val="Arial"/>
       </rPr>
       <t>This event is now closed. Thank you for your interest in Citizenship Day 2024. If you would like to check for other events in your area please visit www.e-immigrate.info</t>
@@ -4600,12 +4592,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="13"/>
-      <color indexed="16"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b val="1"/>
       <sz val="13"/>
       <color indexed="8"/>
@@ -4613,7 +4599,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color indexed="17"/>
+      <color indexed="16"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -4623,25 +4609,31 @@
     </font>
     <font>
       <u val="single"/>
+      <sz val="13"/>
+      <color indexed="17"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u val="single"/>
       <sz val="18"/>
-      <color indexed="16"/>
+      <color indexed="17"/>
       <name val="Arial"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="16"/>
+      <color indexed="17"/>
       <name val="Arial"/>
     </font>
     <font>
       <u val="single"/>
       <sz val="16"/>
-      <color indexed="16"/>
+      <color indexed="17"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="8"/>
-      <color indexed="17"/>
+      <color indexed="16"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -4658,7 +4650,7 @@
     <font>
       <i val="1"/>
       <sz val="10"/>
-      <color indexed="17"/>
+      <color indexed="16"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -5211,7 +5203,7 @@
     <xf numFmtId="49" fontId="10" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="15" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -5289,13 +5281,13 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="18" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="18" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -5421,7 +5413,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -5511,7 +5503,7 @@
     <xf numFmtId="49" fontId="31" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="19" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="18" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -5592,8 +5584,8 @@
       <rgbColor rgb="fff8f9fa"/>
       <rgbColor rgb="ffefefef"/>
       <rgbColor rgb="ff0000ee"/>
+      <rgbColor rgb="ffff0000"/>
       <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffff0000"/>
       <rgbColor rgb="ffffff00"/>
       <rgbColor rgb="ff1155cc"/>
     </indexedColors>
@@ -26899,23 +26891,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B32" r:id="rId1" location="" tooltip="" display="bakLU5yKezs"/>
-    <hyperlink ref="B70" r:id="rId2" location="" tooltip="" display="This event is now closed. Thank you for your interest in Citizenship Day 2024. If you would like to check for other events in your area please visit www.e-immigrate.info"/>
-    <hyperlink ref="C70" r:id="rId3" location="" tooltip="" display="Este evento esta cerrado ahora. Gracias por su interés en el Día de la Ciudadanía 2024. Si desea consultar otros eventos en su área, visite www.e-immigrate.info"/>
-    <hyperlink ref="D70" r:id="rId4" location="" tooltip="" display="Ngày nhập tịch đã đóng. Cảm ơn quý vị đã quan tâm đến ngày Nhập Tịch 2024. Để biết thêm những sự kiện khác trong vùng, xin truy cập trang mạng www.e-immigrate.info"/>
-    <hyperlink ref="E70" r:id="rId5" location="" tooltip="" display="Sarado na po ang kaganapang ito. Salamat po sa iyong interes sa Citizenship Day 2024. Kung gusto ninyong tingnan ang iba pang mga kaganapan sa iyong lugar, mangyaring bisitahin ang www.e-immigrate.info"/>
-    <hyperlink ref="F70" r:id="rId6" location="" tooltip="" display="此活动已经结束。谢谢您对2024年公民日表示兴趣。如果您想查看您的区域内的其他活动，请浏览 www.e-immigrate.info"/>
-    <hyperlink ref="G70" r:id="rId7" location="" tooltip="" display="此活动已经结束。谢谢您对2024年公民日表示兴趣。如果您想查看您的区域内的其他活动，请浏览 www.e-immigrate.info"/>
-    <hyperlink ref="H70" r:id="rId8" location="" tooltip="" display="Мероприятие закрыто. Благодарим за проявленный интерес ко Дню Гражданина 2024. Посетите сайт www.e-immigrate.info, чтобы узнать о других мероприятиях в вашем регионе."/>
-    <hyperlink ref="I70" r:id="rId9" location="" tooltip="" display="በ2024 የዜግነት መርሃ ግብር ላይ ለመሳተፍ ፍላጎት በማሳየትዎ እናመሰግናለን፤፤ ይህ መርሃ ግብር ተጠናቅቆል፥፥ በአካባቢዎ ሊኖሩ ስለሚችሉ ተመሳሳይ ዝግጅቶች ለማወቅ ከፈለጉ ይህንን ድህረ ገፅ ይጎብኙ www.e-immigrate.info"/>
-    <hyperlink ref="J70" r:id="rId10" location="" tooltip="" display="هذا الحدث اصبح ممنتهي االان نشكرا الاهتمامكم في يوم المواطن 2024 أذ كنت ترغب في الاستعلام لاجتماعات اخرى في منطقتك اذهب الى www.e-immigrate.info"/>
-    <hyperlink ref="K70" r:id="rId11" location="" tooltip="" display="این برنامه به پایان رسیده است. از علاقه ی شما به شرکت در برنامه ی سیتیزن شیپی ۲۰۲۳ متشکریم. چنانچه تمایل دارید از سایر برنامه های منطقه ی خود مطلع شوید از وبسایت زیر دیدن فرمایید:www.e-immigrate.info"/>
-    <hyperlink ref="L70" r:id="rId12" location="" tooltip="" display="यह इवेंट अब समापत हो गया है। नागरिकता दिवस 2024 में आपकी रुचि के लिए धन्यवाद। यदि आप अपने क्षेत्र की अन्य घटनाओं की जांच करना चाहते हैं तो कृपया www.e-immigrate.info पर जाएं।"/>
-    <hyperlink ref="M70" r:id="rId13" location="" tooltip="" display="이 이벤트는 이제 종료되었습니다. 2024년 시민권의 날에 관심을 가져주셔서 감사합니다. 해당 지역의 다른 이벤트를 확인하려면 www.e-immigrate.info를 방문하십시오"/>
-    <hyperlink ref="N70" r:id="rId14" location="" tooltip="" display="دا پیښه اوس تړل شوې ده. د تابعیت په ورځ 2024 کې ستاسو د علاقې لپاره مننه. که تاسو غواړئ په خپله سیمه کې د نورو پیښو لپاره وګورئ مهرباني وکړئ www.e-immigrate.info څخه لیدنه وکړئ"/>
-    <hyperlink ref="O70" r:id="rId15" location="" tooltip="" display="ਇਹ ਇਵੈਂਟ ਹੁਣ ਬੰਦ ਹੈ। ਸਿਟੀਜ਼ਨਸ਼ਿਪ ਡੇ 2024 ਵਿੱਚ ਤੁਹਾਡੀ ਦਿਲਚਸਪੀ ਲਈ ਧੰਨਵਾਦ। ਜੇਕਰ ਤੁਸੀਂ ਆਪਣੇ ਖੇਤਰ ਵਿੱਚ ਹੋਰ ਸਮਾਗਮਾਂ ਦੀ ਜਾਂਚ ਕਰਨਾ ਚਾਹੁੰਦੇ ਹੋ ਤਾਂ ਕਿਰਪਾ ਕਰਕੇ www.e-immigrate.info 'ਤੇ ਜਾਓ।"/>
-    <hyperlink ref="P70" r:id="rId16" location="" tooltip="" display="O evento esta encerrado. Obrigado pelo seu interesse no Dia da Cidadania 2024. Para saber informações de outros eventos relacionados a imigração na sua regiao, visite o site www.e-immigrate.info"/>
-    <hyperlink ref="N71" r:id="rId17" location="" tooltip="" display="دا پیښه اوس تړل شوې ده. د تابعیت په ورځ 2024 کې ستاسو د علاقې لپاره مننه. که تاسو غواړئ په خپله سیمه کې د نورو پیښو لپاره وګورئ مهرباني وکړئ www.e-immigrate.info څخه لیدنه وکړئ"/>
+    <hyperlink ref="B70" r:id="rId1" location="" tooltip="" display="This event is now closed. Thank you for your interest in Citizenship Day 2024. If you would like to check for other events in your area please visit www.e-immigrate.info"/>
+    <hyperlink ref="C70" r:id="rId2" location="" tooltip="" display="Este evento esta cerrado ahora. Gracias por su interés en el Día de la Ciudadanía 2024. Si desea consultar otros eventos en su área, visite www.e-immigrate.info"/>
+    <hyperlink ref="D70" r:id="rId3" location="" tooltip="" display="Ngày nhập tịch đã đóng. Cảm ơn quý vị đã quan tâm đến ngày Nhập Tịch 2024. Để biết thêm những sự kiện khác trong vùng, xin truy cập trang mạng www.e-immigrate.info"/>
+    <hyperlink ref="E70" r:id="rId4" location="" tooltip="" display="Sarado na po ang kaganapang ito. Salamat po sa iyong interes sa Citizenship Day 2024. Kung gusto ninyong tingnan ang iba pang mga kaganapan sa iyong lugar, mangyaring bisitahin ang www.e-immigrate.info"/>
+    <hyperlink ref="F70" r:id="rId5" location="" tooltip="" display="此活动已经结束。谢谢您对2024年公民日表示兴趣。如果您想查看您的区域内的其他活动，请浏览 www.e-immigrate.info"/>
+    <hyperlink ref="G70" r:id="rId6" location="" tooltip="" display="此活动已经结束。谢谢您对2024年公民日表示兴趣。如果您想查看您的区域内的其他活动，请浏览 www.e-immigrate.info"/>
+    <hyperlink ref="H70" r:id="rId7" location="" tooltip="" display="Мероприятие закрыто. Благодарим за проявленный интерес ко Дню Гражданина 2024. Посетите сайт www.e-immigrate.info, чтобы узнать о других мероприятиях в вашем регионе."/>
+    <hyperlink ref="I70" r:id="rId8" location="" tooltip="" display="በ2024 የዜግነት መርሃ ግብር ላይ ለመሳተፍ ፍላጎት በማሳየትዎ እናመሰግናለን፤፤ ይህ መርሃ ግብር ተጠናቅቆል፥፥ በአካባቢዎ ሊኖሩ ስለሚችሉ ተመሳሳይ ዝግጅቶች ለማወቅ ከፈለጉ ይህንን ድህረ ገፅ ይጎብኙ www.e-immigrate.info"/>
+    <hyperlink ref="J70" r:id="rId9" location="" tooltip="" display="هذا الحدث اصبح ممنتهي االان نشكرا الاهتمامكم في يوم المواطن 2024 أذ كنت ترغب في الاستعلام لاجتماعات اخرى في منطقتك اذهب الى www.e-immigrate.info"/>
+    <hyperlink ref="K70" r:id="rId10" location="" tooltip="" display="این برنامه به پایان رسیده است. از علاقه ی شما به شرکت در برنامه ی سیتیزن شیپی ۲۰۲۳ متشکریم. چنانچه تمایل دارید از سایر برنامه های منطقه ی خود مطلع شوید از وبسایت زیر دیدن فرمایید:www.e-immigrate.info"/>
+    <hyperlink ref="L70" r:id="rId11" location="" tooltip="" display="यह इवेंट अब समापत हो गया है। नागरिकता दिवस 2024 में आपकी रुचि के लिए धन्यवाद। यदि आप अपने क्षेत्र की अन्य घटनाओं की जांच करना चाहते हैं तो कृपया www.e-immigrate.info पर जाएं।"/>
+    <hyperlink ref="M70" r:id="rId12" location="" tooltip="" display="이 이벤트는 이제 종료되었습니다. 2024년 시민권의 날에 관심을 가져주셔서 감사합니다. 해당 지역의 다른 이벤트를 확인하려면 www.e-immigrate.info를 방문하십시오"/>
+    <hyperlink ref="N70" r:id="rId13" location="" tooltip="" display="دا پیښه اوس تړل شوې ده. د تابعیت په ورځ 2024 کې ستاسو د علاقې لپاره مننه. که تاسو غواړئ په خپله سیمه کې د نورو پیښو لپاره وګورئ مهرباني وکړئ www.e-immigrate.info څخه لیدنه وکړئ"/>
+    <hyperlink ref="O70" r:id="rId14" location="" tooltip="" display="ਇਹ ਇਵੈਂਟ ਹੁਣ ਬੰਦ ਹੈ। ਸਿਟੀਜ਼ਨਸ਼ਿਪ ਡੇ 2024 ਵਿੱਚ ਤੁਹਾਡੀ ਦਿਲਚਸਪੀ ਲਈ ਧੰਨਵਾਦ। ਜੇਕਰ ਤੁਸੀਂ ਆਪਣੇ ਖੇਤਰ ਵਿੱਚ ਹੋਰ ਸਮਾਗਮਾਂ ਦੀ ਜਾਂਚ ਕਰਨਾ ਚਾਹੁੰਦੇ ਹੋ ਤਾਂ ਕਿਰਪਾ ਕਰਕੇ www.e-immigrate.info 'ਤੇ ਜਾਓ।"/>
+    <hyperlink ref="P70" r:id="rId15" location="" tooltip="" display="O evento esta encerrado. Obrigado pelo seu interesse no Dia da Cidadania 2024. Para saber informações de outros eventos relacionados a imigração na sua regiao, visite o site www.e-immigrate.info"/>
+    <hyperlink ref="N71" r:id="rId16" location="" tooltip="" display="دا پیښه اوس تړل شوې ده. د تابعیت په ورځ 2024 کې ستاسو د علاقې لپاره مننه. که تاسو غواړئ په خپله سیمه کې د نورو پیښو لپاره وګورئ مهرباني وکړئ www.e-immigrate.info څخه لیدنه وکړئ"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>